<commit_message>
Fix total expenditure field
In some of the spreadsheets taken from the government, the parsing was corrupted and the total expenditure field did not read (and thus defaulted to 0). This commit fixes that bug, re-running all the data processing as well.
</commit_message>
<xml_diff>
--- a/data/data_clean/2019/GNB2019_bgt_exps.xlsx
+++ b/data/data_clean/2019/GNB2019_bgt_exps.xlsx
@@ -1004,7 +1004,7 @@
         <v>25111970</v>
       </c>
       <c r="P5" s="3">
-        <v>0</v>
+        <v>50223940</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1054,7 +1054,7 @@
         <v>14253139</v>
       </c>
       <c r="P6" s="3">
-        <v>0</v>
+        <v>28506278</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1104,7 +1104,7 @@
         <v>5716131</v>
       </c>
       <c r="P7" s="3">
-        <v>0</v>
+        <v>11432262</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1154,7 +1154,7 @@
         <v>56488232</v>
       </c>
       <c r="P8" s="3">
-        <v>0</v>
+        <v>112976464</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1204,7 +1204,7 @@
         <v>34320084</v>
       </c>
       <c r="P9" s="3">
-        <v>0</v>
+        <v>68640168</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1254,7 +1254,7 @@
         <v>34976767</v>
       </c>
       <c r="P10" s="3">
-        <v>0</v>
+        <v>69953534</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1754,7 +1754,7 @@
         <v>24916144</v>
       </c>
       <c r="P20" s="3">
-        <v>0</v>
+        <v>49832288</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -1804,7 +1804,7 @@
         <v>29416074</v>
       </c>
       <c r="P21" s="3">
-        <v>0</v>
+        <v>58832148</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -1854,7 +1854,7 @@
         <v>17840000</v>
       </c>
       <c r="P22" s="3">
-        <v>0</v>
+        <v>35680000</v>
       </c>
     </row>
     <row r="23" spans="1:16">

</xml_diff>

<commit_message>
Fix total expenditure field (#6)
In some of the spreadsheets taken from the government, the parsing was corrupted and the total expenditure field did not read (and thus defaulted to 0). This commit fixes that bug, re-running all the data processing as well.
</commit_message>
<xml_diff>
--- a/data/data_clean/2019/GNB2019_bgt_exps.xlsx
+++ b/data/data_clean/2019/GNB2019_bgt_exps.xlsx
@@ -1004,7 +1004,7 @@
         <v>25111970</v>
       </c>
       <c r="P5" s="3">
-        <v>0</v>
+        <v>50223940</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1054,7 +1054,7 @@
         <v>14253139</v>
       </c>
       <c r="P6" s="3">
-        <v>0</v>
+        <v>28506278</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1104,7 +1104,7 @@
         <v>5716131</v>
       </c>
       <c r="P7" s="3">
-        <v>0</v>
+        <v>11432262</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1154,7 +1154,7 @@
         <v>56488232</v>
       </c>
       <c r="P8" s="3">
-        <v>0</v>
+        <v>112976464</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1204,7 +1204,7 @@
         <v>34320084</v>
       </c>
       <c r="P9" s="3">
-        <v>0</v>
+        <v>68640168</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1254,7 +1254,7 @@
         <v>34976767</v>
       </c>
       <c r="P10" s="3">
-        <v>0</v>
+        <v>69953534</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1754,7 +1754,7 @@
         <v>24916144</v>
       </c>
       <c r="P20" s="3">
-        <v>0</v>
+        <v>49832288</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -1804,7 +1804,7 @@
         <v>29416074</v>
       </c>
       <c r="P21" s="3">
-        <v>0</v>
+        <v>58832148</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -1854,7 +1854,7 @@
         <v>17840000</v>
       </c>
       <c r="P22" s="3">
-        <v>0</v>
+        <v>35680000</v>
       </c>
     </row>
     <row r="23" spans="1:16">

</xml_diff>